<commit_message>
i changed aveed's kd count
</commit_message>
<xml_diff>
--- a/KD_Count.xlsx
+++ b/KD_Count.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevincho/Desktop/kd_helper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cody/Desktop/kitchen_duty_selector/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A936633-4CB4-0947-BDCD-D52D0E75A276}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B6A3A5-204F-CD42-9ADA-E7E4C137CDB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19420" yWindow="500" windowWidth="16360" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13780" yWindow="460" windowWidth="15020" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -240,14 +240,17 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -499,8 +502,8 @@
   </sheetPr>
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -554,7 +557,7 @@
         <v>47</v>
       </c>
       <c r="B4" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="2">

</xml_diff>